<commit_message>
Implements I/O system for all motors as SparkMax with encoders on Shuffleboard and PID controls
</commit_message>
<xml_diff>
--- a/doc/2020 Pinout.xlsx
+++ b/doc/2020 Pinout.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\blzzrd\git\2020-RobotCode\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FIRSTUser\Git\2020-RobotCode\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8976"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8980"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="111">
   <si>
     <t>left front drive</t>
   </si>
@@ -132,12 +132,237 @@
   </si>
   <si>
     <t>mechanum up/down</t>
+  </si>
+  <si>
+    <t>function</t>
+  </si>
+  <si>
+    <t>device name</t>
+  </si>
+  <si>
+    <t>movement on left front swerve</t>
+  </si>
+  <si>
+    <t>movement on right front swerve</t>
+  </si>
+  <si>
+    <t>movement on left back swerve</t>
+  </si>
+  <si>
+    <t>movement on right back swerve</t>
+  </si>
+  <si>
+    <t>turning on left front swerve</t>
+  </si>
+  <si>
+    <t>turning on right back swerve</t>
+  </si>
+  <si>
+    <t>turning on left back swerve</t>
+  </si>
+  <si>
+    <t>turning on right front swerve</t>
+  </si>
+  <si>
+    <t>spins upper shooter wheels</t>
+  </si>
+  <si>
+    <t>spins lower shooter wheels</t>
+  </si>
+  <si>
+    <t>spins control panel</t>
+  </si>
+  <si>
+    <t>raises and lowers control panel spinning device</t>
+  </si>
+  <si>
+    <t>spins shooter indexer</t>
+  </si>
+  <si>
+    <t>encodes left front drive swerve motor</t>
+  </si>
+  <si>
+    <t>encodes right front drive swerve motor</t>
+  </si>
+  <si>
+    <t>encodes left back drive swerve motor</t>
+  </si>
+  <si>
+    <t>encodes right back drive swerve motor</t>
+  </si>
+  <si>
+    <t>encodes left front turn swerve motor</t>
+  </si>
+  <si>
+    <t>encodes right front turn swerve motor</t>
+  </si>
+  <si>
+    <t>encodes left back turn swerve motor</t>
+  </si>
+  <si>
+    <t>encodes right back turn swerve motor</t>
+  </si>
+  <si>
+    <t>encodes motor for top shooter wheels</t>
+  </si>
+  <si>
+    <t>encodes motor for bottom shooter wheels</t>
+  </si>
+  <si>
+    <t>encodes motor for raising and lowering control panel mechanism</t>
+  </si>
+  <si>
+    <t>encodes motor for shooter indexer</t>
+  </si>
+  <si>
+    <t>measures movement of the robot</t>
+  </si>
+  <si>
+    <t>control panel spin encoder</t>
+  </si>
+  <si>
+    <t>encodes motor for spinning control panel</t>
+  </si>
+  <si>
+    <t>measures color on control panel wheel</t>
+  </si>
+  <si>
+    <t>spins mechanum for ball intake mechanism</t>
+  </si>
+  <si>
+    <t>moves mechanum in alternate direction</t>
+  </si>
+  <si>
+    <t>rotates climber winch to raise robot</t>
+  </si>
+  <si>
+    <t>releases climber after placement</t>
+  </si>
+  <si>
+    <t>measures presence of ball in indexer</t>
+  </si>
+  <si>
+    <t>proposed software names</t>
+  </si>
+  <si>
+    <t>shooterTopWheelMotor</t>
+  </si>
+  <si>
+    <t>swerveLFDMotor</t>
+  </si>
+  <si>
+    <t>swerveRFDMotor</t>
+  </si>
+  <si>
+    <t>swerveLBDMotor</t>
+  </si>
+  <si>
+    <t>swerveRBDMotor</t>
+  </si>
+  <si>
+    <t>swerveLFTMotor</t>
+  </si>
+  <si>
+    <t>swerveRFTMotor</t>
+  </si>
+  <si>
+    <t>swerveLBTMotor</t>
+  </si>
+  <si>
+    <t>swerveRBTMotor</t>
+  </si>
+  <si>
+    <t>shooterBottomWheelMotor</t>
+  </si>
+  <si>
+    <t>shooterIndexerMotor</t>
+  </si>
+  <si>
+    <t>cpanelSpinMotor</t>
+  </si>
+  <si>
+    <t>cpanelElevationMotor</t>
+  </si>
+  <si>
+    <t>climberRelease(Motor)</t>
+  </si>
+  <si>
+    <t>climberWinchAMotor</t>
+  </si>
+  <si>
+    <t>climberWinchBMotor</t>
+  </si>
+  <si>
+    <t>(is it a motor?)</t>
+  </si>
+  <si>
+    <t>(no name due to uncertainty of exact function)</t>
+  </si>
+  <si>
+    <t>(intake i/o starts with intake)</t>
+  </si>
+  <si>
+    <t>swerveLFDEncoder</t>
+  </si>
+  <si>
+    <t>swerveRFDEncoder</t>
+  </si>
+  <si>
+    <t>swerveLBDEncoder</t>
+  </si>
+  <si>
+    <t>swerveRBDEncoder</t>
+  </si>
+  <si>
+    <t>swerveLFTEncoder</t>
+  </si>
+  <si>
+    <t>swerveRFTEncoder</t>
+  </si>
+  <si>
+    <t>swerveLBTEncoder</t>
+  </si>
+  <si>
+    <t>swerveRBTEncoder</t>
+  </si>
+  <si>
+    <t>cpanelColorSensor</t>
+  </si>
+  <si>
+    <t>shooterTopWheelEncoder</t>
+  </si>
+  <si>
+    <t>shooterBottomWheelEncoder</t>
+  </si>
+  <si>
+    <t>cpanelElevationEncoder</t>
+  </si>
+  <si>
+    <t>cpanelSpinEncoder</t>
+  </si>
+  <si>
+    <t>shooterIndexerEncoder</t>
+  </si>
+  <si>
+    <t>(format is system Function Item)</t>
+  </si>
+  <si>
+    <t>shooterBallSensor</t>
+  </si>
+  <si>
+    <t>robotGyroSensor</t>
+  </si>
+  <si>
+    <t>shooterIntakeMotor</t>
+  </si>
+  <si>
+    <t>shooterIntakeElevationMotor</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -458,201 +683,434 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:A39"/>
+  <dimension ref="A2:E40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="21.47265625" customWidth="1"/>
-    <col min="2" max="2" width="17.68359375" customWidth="1"/>
+    <col min="1" max="1" width="27" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.6328125" customWidth="1"/>
+    <col min="3" max="3" width="55.90625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="40.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="C3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" t="s">
+        <v>74</v>
+      </c>
+      <c r="E3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="C4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="C5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="C6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D6" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="C7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D7" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="C8" t="s">
+        <v>45</v>
+      </c>
+      <c r="D8" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="C9" t="s">
+        <v>44</v>
+      </c>
+      <c r="D9" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="C10" t="s">
+        <v>43</v>
+      </c>
+      <c r="D10" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="C11" t="s">
+        <v>46</v>
+      </c>
+      <c r="D11" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="C12" t="s">
+        <v>47</v>
+      </c>
+      <c r="D12" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="C13" t="s">
+        <v>50</v>
+      </c>
+      <c r="D13" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="C14" t="s">
+        <v>67</v>
+      </c>
+      <c r="D14" t="s">
+        <v>109</v>
+      </c>
+      <c r="E14" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="C15" t="s">
+        <v>48</v>
+      </c>
+      <c r="D15" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="C16" t="s">
+        <v>49</v>
+      </c>
+      <c r="D16" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="C17" t="s">
+        <v>70</v>
+      </c>
+      <c r="D17" t="s">
+        <v>86</v>
+      </c>
+      <c r="E17" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="C18" t="s">
+        <v>69</v>
+      </c>
+      <c r="D18" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="C19" t="s">
+        <v>69</v>
+      </c>
+      <c r="D19" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="C20" t="s">
+        <v>68</v>
+      </c>
+      <c r="D20" t="s">
+        <v>110</v>
+      </c>
+      <c r="E20" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="C23" t="s">
+        <v>51</v>
+      </c>
+      <c r="D23" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="C24" t="s">
+        <v>52</v>
+      </c>
+      <c r="D24" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="C25" t="s">
+        <v>53</v>
+      </c>
+      <c r="D25" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="C26" t="s">
+        <v>54</v>
+      </c>
+      <c r="D26" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="C27" t="s">
+        <v>55</v>
+      </c>
+      <c r="D27" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="C28" t="s">
+        <v>56</v>
+      </c>
+      <c r="D28" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="C29" t="s">
+        <v>57</v>
+      </c>
+      <c r="D29" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="C30" t="s">
+        <v>58</v>
+      </c>
+      <c r="D30" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="C31" t="s">
+        <v>66</v>
+      </c>
+      <c r="D31" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="C32" t="s">
+        <v>71</v>
+      </c>
+      <c r="D32" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="C34" t="s">
+        <v>59</v>
+      </c>
+      <c r="D34" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="C35" t="s">
+        <v>60</v>
+      </c>
+      <c r="D35" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="C36" t="s">
+        <v>61</v>
+      </c>
+      <c r="D36" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="C38" t="s">
+        <v>62</v>
+      </c>
+      <c r="D38" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>34</v>
+      </c>
+      <c r="C39" t="s">
+        <v>63</v>
+      </c>
+      <c r="D39" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>64</v>
+      </c>
+      <c r="C40" t="s">
+        <v>65</v>
+      </c>
+      <c r="D40" t="s">
+        <v>104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>